<commit_message>
Simplify section level handling
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/multiple_column_names.xlsx
+++ b/tests/integration_test_files/multiple_column_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240547B2-72FA-C944-8A6D-488889F63772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD38142-5542-BF47-87D0-91325E9A75E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="64600" yWindow="740" windowWidth="33000" windowHeight="22600" activeTab="9" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="67600" yWindow="500" windowWidth="33000" windowHeight="22600" firstSheet="7" activeTab="14" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="566">
   <si>
     <t>Epoch</t>
   </si>
@@ -1538,15 +1538,6 @@
     <t>&lt;p&gt;Blinding and unblinding text here please&lt;/p&gt;</t>
   </si>
   <si>
-    <t>sectionNumber1</t>
-  </si>
-  <si>
-    <t>sectionNumber2</t>
-  </si>
-  <si>
-    <t>sectionNumber3</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -1683,6 +1674,90 @@
   </si>
   <si>
     <t>Old population</t>
+  </si>
+  <si>
+    <t>sectionNumber</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>7.3</t>
+  </si>
+  <si>
+    <t>7.4</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>8.4</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>8.6</t>
+  </si>
+  <si>
+    <t>8.7</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>8.9</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>9.3</t>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>9.6</t>
+  </si>
+  <si>
+    <t>9.7</t>
+  </si>
+  <si>
+    <t>9.8</t>
+  </si>
+  <si>
+    <t>9.9</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>10.2</t>
+  </si>
+  <si>
+    <t>10.3</t>
+  </si>
+  <si>
+    <t>10.4</t>
+  </si>
+  <si>
+    <t>10.5</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1766,7 +1841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1841,17 +1916,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2460,7 +2532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2473,7 +2545,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>84</v>
@@ -3352,1294 +3424,1232 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="16" style="3" customWidth="1"/>
-    <col min="5" max="5" width="49.83203125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="81.33203125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="16" style="3" customWidth="1"/>
+    <col min="3" max="3" width="49.83203125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="81.33203125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
+        <v>538</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>492</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="C1" s="27" t="s">
+        <v>286</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>423</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>427</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>429</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="10" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="10" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="10" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>515</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="10" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>516</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="C18" s="10" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="B19" s="28"/>
+      <c r="C19" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="B20" s="28"/>
+      <c r="C20" s="10" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>518</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="10" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>519</v>
+      </c>
+      <c r="B22" s="28"/>
+      <c r="C22" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="B23" s="28"/>
+      <c r="C23" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="B25" s="28"/>
+      <c r="C25" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>483</v>
+      </c>
+      <c r="B26" s="28"/>
+      <c r="C26" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="B27" s="28"/>
+      <c r="C27" s="10" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="C28" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="B29" s="28"/>
+      <c r="C29" s="10" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
         <v>494</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="B30" s="28"/>
+      <c r="C30" s="10" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="B32" s="28"/>
+      <c r="C32" s="10" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>525</v>
+      </c>
+      <c r="B33" s="28"/>
+      <c r="C33" s="10" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="B34" s="28"/>
+      <c r="C34" s="10" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>526</v>
+      </c>
+      <c r="B35" s="28"/>
+      <c r="C35" s="10" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="B36" s="28"/>
+      <c r="C36" s="10" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="B37" s="28"/>
+      <c r="C37" s="10" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="B38" s="28"/>
+      <c r="C38" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="B39" s="28"/>
+      <c r="C39" s="10" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>528</v>
+      </c>
+      <c r="B40" s="28"/>
+      <c r="C40" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="B41" s="28"/>
+      <c r="C41" s="10" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="B42" s="28"/>
+      <c r="C42" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="B43" s="28"/>
+      <c r="C43" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>529</v>
+      </c>
+      <c r="B44" s="28"/>
+      <c r="C44" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="B45" s="28"/>
+      <c r="C45" s="10" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="B46" s="28"/>
+      <c r="C46" s="10" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="B47" s="28"/>
+      <c r="C47" s="10" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="B48" s="28"/>
+      <c r="C48" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="B49" s="28"/>
+      <c r="C49" s="10" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
         <v>495</v>
       </c>
-      <c r="E1" s="27" t="s">
-        <v>286</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="10" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B3" s="28" t="s">
-        <v>421</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B4" s="28" t="s">
-        <v>422</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B5" s="28" t="s">
-        <v>423</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
-        <v>424</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="E6" s="10" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B7" s="28" t="s">
-        <v>425</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B8" s="28" t="s">
-        <v>426</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
-        <v>427</v>
-      </c>
-      <c r="B9" s="28"/>
-      <c r="E9" s="10" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
-        <v>428</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="E10" s="10" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B11" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C12" s="30" t="s">
-        <v>420</v>
-      </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="10" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="28" t="s">
-        <v>430</v>
-      </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="10" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C14" s="30" t="s">
-        <v>431</v>
-      </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="10" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C15" s="30" t="s">
-        <v>432</v>
-      </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="10" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C16" s="30" t="s">
-        <v>433</v>
-      </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="10" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B17" s="30" t="s">
-        <v>518</v>
-      </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="10" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B18" s="30" t="s">
-        <v>519</v>
-      </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="10" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
+      <c r="B50" s="28"/>
+      <c r="C50" s="10" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="11" t="s">
+        <v>531</v>
+      </c>
+      <c r="B51" s="28"/>
+      <c r="C51" s="10" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A52" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="B52" s="28"/>
+      <c r="C52" s="10" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A53" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="B53" s="28"/>
+      <c r="C53" s="10" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="B54" s="28"/>
+      <c r="C54" s="10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="B55" s="28"/>
+      <c r="C55" s="10" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="11" t="s">
+        <v>540</v>
+      </c>
+      <c r="B56" s="28"/>
+      <c r="C56" s="10" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="B57" s="28"/>
+      <c r="C57" s="10" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="11" t="s">
         <v>496</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="10" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B20" s="30" t="s">
-        <v>520</v>
-      </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="10" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B21" s="30" t="s">
-        <v>521</v>
-      </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="10" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="B22" s="30" t="s">
-        <v>522</v>
-      </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="B23" s="30" t="s">
-        <v>523</v>
-      </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B24" s="30" t="s">
-        <v>524</v>
-      </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="10" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B25" s="28"/>
-      <c r="C25" s="30" t="s">
-        <v>482</v>
-      </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="10" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B26" s="28"/>
-      <c r="C26" s="30" t="s">
-        <v>483</v>
-      </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="10" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B27" s="28"/>
-      <c r="C27" s="30" t="s">
-        <v>484</v>
-      </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="10" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B28" s="28"/>
-      <c r="C28" s="30" t="s">
-        <v>485</v>
-      </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="10" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B29" s="30" t="s">
-        <v>525</v>
-      </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="10" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="30" t="s">
+      <c r="B58" s="28"/>
+      <c r="C58" s="10" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="B59" s="28"/>
+      <c r="C59" s="10" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="B60" s="28"/>
+      <c r="C60" s="10" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="B61" s="28"/>
+      <c r="C61" s="10" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="11" t="s">
+        <v>486</v>
+      </c>
+      <c r="B62" s="28"/>
+      <c r="C62" s="10" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="B63" s="28"/>
+      <c r="C63" s="10" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="B64" s="28"/>
+      <c r="C64" s="10" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="B65" s="28"/>
+      <c r="C65" s="10" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="B66" s="28"/>
+      <c r="C66" s="10" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="11" t="s">
+        <v>545</v>
+      </c>
+      <c r="B67" s="28"/>
+      <c r="C67" s="10" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="B68" s="28"/>
+      <c r="C68" s="10" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A69" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="B69" s="28"/>
+      <c r="C69" s="10" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="B70" s="28"/>
+      <c r="C70" s="10" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="B71" s="28"/>
+      <c r="C71" s="10" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" s="11" t="s">
+        <v>461</v>
+      </c>
+      <c r="B72" s="28"/>
+      <c r="C72" s="10" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="B73" s="28"/>
+      <c r="C73" s="10" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="11" t="s">
+        <v>463</v>
+      </c>
+      <c r="B74" s="28"/>
+      <c r="C74" s="10" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="B75" s="28"/>
+      <c r="C75" s="10" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="B76" s="28"/>
+      <c r="C76" s="10" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A77" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="B77" s="28"/>
+      <c r="C77" s="10" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="11" t="s">
+        <v>546</v>
+      </c>
+      <c r="B78" s="28"/>
+      <c r="C78" s="10" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="11" t="s">
+        <v>467</v>
+      </c>
+      <c r="B79" s="28"/>
+      <c r="C79" s="10" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="B80" s="28"/>
+      <c r="C80" s="10" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A81" s="11" t="s">
+        <v>547</v>
+      </c>
+      <c r="B81" s="28"/>
+      <c r="C81" s="10" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="B82" s="28"/>
+      <c r="C82" s="10" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="B83" s="28"/>
+      <c r="C83" s="10" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A84" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="B84" s="28"/>
+      <c r="C84" s="10" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="B85" s="28"/>
+      <c r="C85" s="10" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A86" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="B86" s="28"/>
+      <c r="C86" s="10" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="11" t="s">
+        <v>548</v>
+      </c>
+      <c r="B87" s="28"/>
+      <c r="C87" s="10" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A88" s="11" t="s">
+        <v>549</v>
+      </c>
+      <c r="B88" s="28"/>
+      <c r="C88" s="10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" s="11" t="s">
+        <v>550</v>
+      </c>
+      <c r="B89" s="28"/>
+      <c r="C89" s="10" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A90" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="B90" s="28"/>
+      <c r="C90" s="10" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="B91" s="28"/>
+      <c r="C91" s="10" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A92" s="11" t="s">
         <v>497</v>
       </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="10" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B31" s="30" t="s">
-        <v>526</v>
-      </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B32" s="30" t="s">
-        <v>527</v>
-      </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="10" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B33" s="30" t="s">
-        <v>528</v>
-      </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="10" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C34" s="30" t="s">
-        <v>438</v>
-      </c>
-      <c r="D34" s="28"/>
-      <c r="E34" s="10" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B35" s="30" t="s">
-        <v>529</v>
-      </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="10" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B36" s="30" t="s">
-        <v>530</v>
-      </c>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="10" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C37" s="30" t="s">
-        <v>439</v>
-      </c>
-      <c r="D37" s="28"/>
-      <c r="E37" s="10" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C38" s="30" t="s">
-        <v>440</v>
-      </c>
-      <c r="D38" s="28"/>
-      <c r="E38" s="10" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C39" s="30" t="s">
-        <v>441</v>
-      </c>
-      <c r="D39" s="28"/>
-      <c r="E39" s="10" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B40" s="30" t="s">
-        <v>531</v>
-      </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="10" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C41" s="30" t="s">
-        <v>442</v>
-      </c>
-      <c r="D41" s="28"/>
-      <c r="E41" s="10" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C42" s="30" t="s">
-        <v>443</v>
-      </c>
-      <c r="D42" s="28"/>
-      <c r="E42" s="10" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C43" s="30" t="s">
-        <v>444</v>
-      </c>
-      <c r="D43" s="28"/>
-      <c r="E43" s="10" t="s">
-        <v>329</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B44" s="30" t="s">
-        <v>532</v>
-      </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="10" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B45" s="30" t="s">
-        <v>533</v>
-      </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="10" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C46" s="30" t="s">
-        <v>445</v>
-      </c>
-      <c r="D46" s="28"/>
-      <c r="E46" s="10" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C47" s="30" t="s">
-        <v>446</v>
-      </c>
-      <c r="D47" s="28"/>
-      <c r="E47" s="10" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C48" s="30" t="s">
-        <v>447</v>
-      </c>
-      <c r="D48" s="28"/>
-      <c r="E48" s="10" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C49" s="30" t="s">
-        <v>448</v>
-      </c>
-      <c r="D49" s="28"/>
-      <c r="E49" s="10" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A50" s="30" t="s">
+      <c r="B92" s="28"/>
+      <c r="C92" s="10" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="11" t="s">
+        <v>551</v>
+      </c>
+      <c r="B93" s="28"/>
+      <c r="C93" s="10" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" s="11" t="s">
+        <v>552</v>
+      </c>
+      <c r="B94" s="28"/>
+      <c r="C94" s="10" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" s="11" t="s">
+        <v>474</v>
+      </c>
+      <c r="B95" s="28"/>
+      <c r="C95" s="10" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="B96" s="28"/>
+      <c r="C96" s="10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="B97" s="28"/>
+      <c r="C97" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="11" t="s">
+        <v>477</v>
+      </c>
+      <c r="B98" s="28"/>
+      <c r="C98" s="10" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="11" t="s">
+        <v>478</v>
+      </c>
+      <c r="B99" s="28"/>
+      <c r="C99" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="11" t="s">
+        <v>553</v>
+      </c>
+      <c r="B100" s="28"/>
+      <c r="C100" s="10" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="11" t="s">
+        <v>554</v>
+      </c>
+      <c r="B101" s="28"/>
+      <c r="C101" s="10" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="11" t="s">
+        <v>555</v>
+      </c>
+      <c r="B102" s="28"/>
+      <c r="C102" s="10" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="11" t="s">
+        <v>556</v>
+      </c>
+      <c r="B103" s="28"/>
+      <c r="C103" s="10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="11" t="s">
+        <v>557</v>
+      </c>
+      <c r="B104" s="28"/>
+      <c r="C104" s="10" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="11" t="s">
+        <v>558</v>
+      </c>
+      <c r="B105" s="28"/>
+      <c r="C105" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" s="11" t="s">
+        <v>559</v>
+      </c>
+      <c r="B106" s="28"/>
+      <c r="C106" s="10" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A107" s="11" t="s">
         <v>498</v>
       </c>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="10" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B51" s="30" t="s">
-        <v>534</v>
-      </c>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="10" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="C52" s="28" t="s">
-        <v>449</v>
-      </c>
-      <c r="D52" s="28"/>
-      <c r="E52" s="10" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="C53" s="28" t="s">
-        <v>450</v>
-      </c>
-      <c r="D53" s="28"/>
-      <c r="E53" s="10" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C54" s="28" t="s">
-        <v>451</v>
-      </c>
-      <c r="D54" s="28"/>
-      <c r="E54" s="10" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B55" s="28">
-        <v>7.2</v>
-      </c>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="10" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B56" s="28">
-        <v>7.3</v>
-      </c>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="10" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B57" s="28">
-        <v>7.4</v>
-      </c>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="10" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="30" t="s">
+      <c r="B107" s="28"/>
+      <c r="C107" s="10" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="11" t="s">
+        <v>560</v>
+      </c>
+      <c r="B108" s="28"/>
+      <c r="C108" s="10" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="11" t="s">
+        <v>561</v>
+      </c>
+      <c r="B109" s="28"/>
+      <c r="C109" s="10" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="11" t="s">
+        <v>562</v>
+      </c>
+      <c r="B110" s="28"/>
+      <c r="C110" s="10" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="11" t="s">
+        <v>563</v>
+      </c>
+      <c r="B111" s="28"/>
+      <c r="C111" s="10" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="11" t="s">
+        <v>564</v>
+      </c>
+      <c r="B112" s="28"/>
+      <c r="C112" s="10" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A113" s="11" t="s">
         <v>499</v>
       </c>
-      <c r="B58" s="28"/>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="10" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B59" s="28">
-        <v>8.1</v>
-      </c>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="10" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B60" s="28">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="C60" s="28"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="10" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B61" s="28">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="10" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C62" s="28" t="s">
-        <v>486</v>
-      </c>
-      <c r="D62" s="28"/>
-      <c r="E62" s="10" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C63" s="28" t="s">
-        <v>453</v>
-      </c>
-      <c r="D63" s="28"/>
-      <c r="E63" s="10" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C64" s="28" t="s">
-        <v>454</v>
-      </c>
-      <c r="D64" s="28"/>
-      <c r="E64" s="10" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C65" s="28" t="s">
-        <v>455</v>
-      </c>
-      <c r="D65" s="28"/>
-      <c r="E65" s="10" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C66" s="28" t="s">
-        <v>456</v>
-      </c>
-      <c r="D66" s="28"/>
-      <c r="E66" s="10" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B67" s="28">
-        <v>8.4</v>
-      </c>
-      <c r="C67" s="28"/>
-      <c r="D67" s="28"/>
-      <c r="E67" s="10" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C68" s="28" t="s">
-        <v>487</v>
-      </c>
-      <c r="D68" s="28"/>
-      <c r="E68" s="10" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="C69" s="28" t="s">
-        <v>458</v>
-      </c>
-      <c r="D69" s="28"/>
-      <c r="E69" s="10" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C70" s="28" t="s">
-        <v>459</v>
-      </c>
-      <c r="D70" s="28"/>
-      <c r="E70" s="10" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C71" s="28" t="s">
-        <v>460</v>
-      </c>
-      <c r="D71" s="28"/>
-      <c r="E71" s="10" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C72" s="28" t="s">
-        <v>461</v>
-      </c>
-      <c r="D72" s="28"/>
-      <c r="E72" s="10" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C73" s="28" t="s">
-        <v>462</v>
-      </c>
-      <c r="D73" s="28"/>
-      <c r="E73" s="10" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C74" s="28" t="s">
-        <v>463</v>
-      </c>
-      <c r="D74" s="28"/>
-      <c r="E74" s="10" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C75" s="28" t="s">
-        <v>464</v>
-      </c>
-      <c r="D75" s="28"/>
-      <c r="E75" s="10" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C76" s="28" t="s">
-        <v>465</v>
-      </c>
-      <c r="D76" s="28"/>
-      <c r="E76" s="10" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="C77" s="28" t="s">
-        <v>466</v>
-      </c>
-      <c r="D77" s="28"/>
-      <c r="E77" s="10" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B78" s="28">
-        <v>8.5</v>
-      </c>
-      <c r="C78" s="28"/>
-      <c r="D78" s="28"/>
-      <c r="E78" s="10" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C79" s="28" t="s">
-        <v>467</v>
-      </c>
-      <c r="D79" s="28"/>
-      <c r="E79" s="10" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C80" s="28" t="s">
-        <v>468</v>
-      </c>
-      <c r="D80" s="28"/>
-      <c r="E80" s="10" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="B81" s="28">
-        <v>8.6</v>
-      </c>
-      <c r="C81" s="28"/>
-      <c r="D81" s="28"/>
-      <c r="E81" s="10" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C82" s="28" t="s">
-        <v>469</v>
-      </c>
-      <c r="D82" s="28"/>
-      <c r="E82" s="10" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C83" s="28" t="s">
-        <v>470</v>
-      </c>
-      <c r="D83" s="28"/>
-      <c r="E83" s="10" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="C84" s="28" t="s">
-        <v>471</v>
-      </c>
-      <c r="D84" s="28"/>
-      <c r="E84" s="10" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C85" s="28" t="s">
-        <v>472</v>
-      </c>
-      <c r="D85" s="28"/>
-      <c r="E85" s="10" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="C86" s="28" t="s">
-        <v>473</v>
-      </c>
-      <c r="D86" s="28"/>
-      <c r="E86" s="10" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B87" s="28">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="C87" s="28"/>
-      <c r="D87" s="28"/>
-      <c r="E87" s="10" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B88" s="28">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C88" s="28"/>
-      <c r="D88" s="28"/>
-      <c r="E88" s="10" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B89" s="28">
-        <v>8.9</v>
-      </c>
-      <c r="C89" s="28"/>
-      <c r="D89" s="28"/>
-      <c r="E89" s="10" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B90" s="28">
-        <v>8.1</v>
-      </c>
-      <c r="C90" s="28"/>
-      <c r="D90" s="28"/>
-      <c r="E90" s="10" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C91" s="28" t="s">
-        <v>488</v>
-      </c>
-      <c r="D91" s="28"/>
-      <c r="E91" s="10" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="30" t="s">
+      <c r="B113" s="28"/>
+      <c r="C113" s="10" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" s="11" t="s">
+        <v>514</v>
+      </c>
+      <c r="B114" s="28"/>
+      <c r="C114" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="B115" s="28"/>
+      <c r="C115" s="10" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="11" t="s">
+        <v>512</v>
+      </c>
+      <c r="B116" s="28"/>
+      <c r="C116" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A117" s="11" t="s">
         <v>500</v>
       </c>
-      <c r="B92" s="28"/>
-      <c r="C92" s="28"/>
-      <c r="D92" s="28"/>
-      <c r="E92" s="10" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B93" s="28">
-        <v>9.1</v>
-      </c>
-      <c r="C93" s="28"/>
-      <c r="D93" s="28"/>
-      <c r="E93" s="10" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B94" s="28">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="C94" s="28"/>
-      <c r="D94" s="28"/>
-      <c r="E94" s="10" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C95" s="28" t="s">
-        <v>474</v>
-      </c>
-      <c r="D95" s="28"/>
-      <c r="E95" s="10" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C96" s="28" t="s">
-        <v>475</v>
-      </c>
-      <c r="D96" s="28"/>
-      <c r="E96" s="10" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C97" s="28" t="s">
-        <v>476</v>
-      </c>
-      <c r="D97" s="28"/>
-      <c r="E97" s="10" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C98" s="28" t="s">
-        <v>477</v>
-      </c>
-      <c r="D98" s="28"/>
-      <c r="E98" s="10" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C99" s="28" t="s">
-        <v>478</v>
-      </c>
-      <c r="D99" s="28"/>
-      <c r="E99" s="10" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B100" s="28">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="C100" s="28"/>
-      <c r="D100" s="28"/>
-      <c r="E100" s="10" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B101" s="28">
-        <v>9.4</v>
-      </c>
-      <c r="C101" s="28"/>
-      <c r="D101" s="28"/>
-      <c r="E101" s="10" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B102" s="28">
-        <v>9.5</v>
-      </c>
-      <c r="C102" s="28"/>
-      <c r="D102" s="28"/>
-      <c r="E102" s="10" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B103" s="28">
-        <v>9.6</v>
-      </c>
-      <c r="C103" s="28"/>
-      <c r="D103" s="28"/>
-      <c r="E103" s="10" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B104" s="28">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="C104" s="28"/>
-      <c r="D104" s="28"/>
-      <c r="E104" s="10" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B105" s="28">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="C105" s="28"/>
-      <c r="D105" s="28"/>
-      <c r="E105" s="10" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B106" s="28">
-        <v>9.9</v>
-      </c>
-      <c r="C106" s="28"/>
-      <c r="D106" s="28"/>
-      <c r="E106" s="10" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A107" s="30" t="s">
+      <c r="B117" s="28"/>
+      <c r="C117" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="B118" s="28"/>
+      <c r="C118" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A119" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="B119" s="28"/>
+      <c r="C119" s="10" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="11" t="s">
+        <v>509</v>
+      </c>
+      <c r="B120" s="28"/>
+      <c r="C120" s="10" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="11" t="s">
+        <v>508</v>
+      </c>
+      <c r="B121" s="28"/>
+      <c r="C121" s="10" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A122" s="11" t="s">
         <v>501</v>
       </c>
-      <c r="B107" s="28"/>
-      <c r="C107" s="28"/>
-      <c r="D107" s="28"/>
-      <c r="E107" s="10" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B108" s="28">
-        <v>10.1</v>
-      </c>
-      <c r="C108" s="28"/>
-      <c r="D108" s="28"/>
-      <c r="E108" s="10" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B109" s="28">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="C109" s="28"/>
-      <c r="D109" s="28"/>
-      <c r="E109" s="10" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B110" s="28">
-        <v>10.3</v>
-      </c>
-      <c r="C110" s="28"/>
-      <c r="D110" s="28"/>
-      <c r="E110" s="10" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B111" s="28">
-        <v>10.4</v>
-      </c>
-      <c r="C111" s="28"/>
-      <c r="D111" s="28"/>
-      <c r="E111" s="10" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B112" s="28">
-        <v>10.5</v>
-      </c>
-      <c r="C112" s="28"/>
-      <c r="D112" s="28"/>
-      <c r="E112" s="10" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A113" s="30" t="s">
+      <c r="B122" s="28"/>
+      <c r="C122" s="10" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A123" s="11" t="s">
+        <v>507</v>
+      </c>
+      <c r="B123" s="28"/>
+      <c r="C123" s="10" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A124" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="B124" s="28"/>
+      <c r="C124" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A125" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="B125" s="28"/>
+      <c r="C125" s="10" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A126" s="11" t="s">
+        <v>481</v>
+      </c>
+      <c r="B126" s="28"/>
+      <c r="C126" s="10" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A127" s="11" t="s">
+        <v>506</v>
+      </c>
+      <c r="B127" s="28"/>
+      <c r="C127" s="10" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A128" s="11" t="s">
+        <v>505</v>
+      </c>
+      <c r="B128" s="28"/>
+      <c r="C128" s="10" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A129" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="B129" s="28"/>
+      <c r="C129" s="10" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A130" s="11" t="s">
         <v>502</v>
       </c>
-      <c r="B113" s="28"/>
-      <c r="C113" s="28"/>
-      <c r="D113" s="28"/>
-      <c r="E113" s="10" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B114" s="30" t="s">
-        <v>517</v>
-      </c>
-      <c r="C114" s="28"/>
-      <c r="D114" s="28"/>
-      <c r="E114" s="10" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B115" s="30" t="s">
-        <v>516</v>
-      </c>
-      <c r="C115" s="28"/>
-      <c r="D115" s="28"/>
-      <c r="E115" s="10" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B116" s="30" t="s">
-        <v>515</v>
-      </c>
-      <c r="C116" s="28"/>
-      <c r="D116" s="28"/>
-      <c r="E116" s="10" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A117" s="30" t="s">
+      <c r="B130" s="28"/>
+      <c r="C130" s="10" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A131" s="11" t="s">
         <v>503</v>
       </c>
-      <c r="B117" s="28"/>
-      <c r="C117" s="28"/>
-      <c r="D117" s="28"/>
-      <c r="E117" s="10" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B118" s="30" t="s">
-        <v>514</v>
-      </c>
-      <c r="C118" s="28"/>
-      <c r="D118" s="28"/>
-      <c r="E118" s="10" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B119" s="30" t="s">
-        <v>513</v>
-      </c>
-      <c r="C119" s="28"/>
-      <c r="D119" s="28"/>
-      <c r="E119" s="10" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B120" s="30" t="s">
-        <v>512</v>
-      </c>
-      <c r="C120" s="28"/>
-      <c r="D120" s="28"/>
-      <c r="E120" s="10" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B121" s="30" t="s">
-        <v>511</v>
-      </c>
-      <c r="C121" s="28"/>
-      <c r="D121" s="28"/>
-      <c r="E121" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A122" s="30" t="s">
-        <v>504</v>
-      </c>
-      <c r="B122" s="28"/>
-      <c r="C122" s="28"/>
-      <c r="D122" s="28"/>
-      <c r="E122" s="10" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B123" s="30" t="s">
-        <v>510</v>
-      </c>
-      <c r="C123" s="28"/>
-      <c r="D123" s="28"/>
-      <c r="E123" s="10" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C124" s="30" t="s">
-        <v>479</v>
-      </c>
-      <c r="D124" s="28"/>
-      <c r="E124" s="10" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C125" s="30" t="s">
-        <v>480</v>
-      </c>
-      <c r="D125" s="28"/>
-      <c r="E125" s="10" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C126" s="30" t="s">
-        <v>481</v>
-      </c>
-      <c r="D126" s="28"/>
-      <c r="E126" s="10" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B127" s="30" t="s">
-        <v>509</v>
-      </c>
-      <c r="C127" s="28"/>
-      <c r="D127" s="28"/>
-      <c r="E127" s="10" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B128" s="30" t="s">
-        <v>508</v>
-      </c>
-      <c r="C128" s="28"/>
-      <c r="D128" s="28"/>
-      <c r="E128" s="10" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B129" s="30" t="s">
-        <v>507</v>
-      </c>
-      <c r="C129" s="28"/>
-      <c r="D129" s="28"/>
-      <c r="E129" s="10" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A130" s="30" t="s">
-        <v>505</v>
-      </c>
-      <c r="B130" s="28"/>
-      <c r="C130" s="28"/>
-      <c r="D130" s="28"/>
-      <c r="E130" s="10" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A131" s="30" t="s">
-        <v>506</v>
-      </c>
       <c r="B131" s="28"/>
-      <c r="C131" s="28"/>
-      <c r="D131" s="28"/>
-      <c r="E131" s="10" t="s">
+      <c r="C131" s="10" t="s">
         <v>418</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="11" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="11" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="11" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="11" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="11" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="11" t="s">
+        <v>565</v>
       </c>
     </row>
   </sheetData>
@@ -6644,34 +6654,34 @@
       <c r="A1" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>249</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
@@ -6699,54 +6709,54 @@
       <c r="A6" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
@@ -6813,16 +6823,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7015,10 +7025,10 @@
       <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="34"/>
+      <c r="G1" s="33"/>
       <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
@@ -7422,7 +7432,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>64</v>
@@ -7444,10 +7454,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="B2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -7464,10 +7474,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B3" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -7484,10 +7494,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>534</v>
+      </c>
+      <c r="B4" t="s">
         <v>537</v>
-      </c>
-      <c r="B4" t="s">
-        <v>540</v>
       </c>
       <c r="C4">
         <v>20</v>

</xml_diff>